<commit_message>
Download videos, simplyfy paths
</commit_message>
<xml_diff>
--- a/eye_preproc/Organize/file_order.xlsx
+++ b/eye_preproc/Organize/file_order.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">inscapes</t>
   </si>
   <si>
-    <t xml:space="preserve">Inscapes_02.mp4</t>
+    <t xml:space="preserve">Inscapes_02.avi</t>
   </si>
   <si>
     <t xml:space="preserve">_R01_ThePresent_ScannerON</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">the_present</t>
   </si>
   <si>
-    <t xml:space="preserve">The_Present.mp4</t>
+    <t xml:space="preserve">The_Present_720x480.avi</t>
   </si>
   <si>
     <t xml:space="preserve">_R02_ThePresent_ScannerON</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">despicable_me_eng</t>
   </si>
   <si>
-    <t xml:space="preserve">Despicable_Me_English.mp4</t>
+    <t xml:space="preserve">Despicable_Me_720x480_English.avi</t>
   </si>
   <si>
     <t xml:space="preserve">_R02_DespicableMeEng_ScannerON</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">despicable_me_hun</t>
   </si>
   <si>
-    <t xml:space="preserve">Despicable_Me_Hungarian.mp4</t>
+    <t xml:space="preserve">Despicable_Me_720x480_Hungarian.avi</t>
   </si>
   <si>
     <t xml:space="preserve">_R02_DespicableMeHun_ScannerON</t>
@@ -332,10 +332,10 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.13"/>

</xml_diff>